<commit_message>
Update WrittenMarkImport and WrittenMarkImportController for improved data handling; change 'from_number' to 'roll_number' and implement updateOrInsert for better record management.
</commit_message>
<xml_diff>
--- a/public/uploads/written-exam-import.xlsx
+++ b/public/uploads/written-exam-import.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{433DD830-3D16-42EF-875F-545F5FF353D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,9 +17,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>from_number</t>
-  </si>
-  <si>
     <t>bangla</t>
   </si>
   <si>
@@ -32,12 +30,15 @@
   </si>
   <si>
     <t>gk</t>
+  </si>
+  <si>
+    <t>roll_number</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -79,7 +80,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -95,9 +96,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -135,9 +136,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -172,7 +173,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -207,7 +208,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -380,11 +381,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -399,22 +400,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>